<commit_message>
Corrected name of directory (Warr2010 --> Warr2000)
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/Econ2011/AllDataWorkbook.xlsx
+++ b/data/Excel Workbooks/Econ2011/AllDataWorkbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="555" yWindow="555" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28100" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
   </externalReferences>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,9 +30,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="3">
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Econ2011</t>
   </si>
 </sst>
 </file>
@@ -114,7 +120,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="United States Workbook"/>
@@ -1102,7 +1108,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="UK Workbook"/>
@@ -2064,7 +2070,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Japan Workbook"/>
@@ -3024,7 +3030,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="China Workbook"/>
@@ -3655,7 +3661,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="South Africa Workbook"/>
@@ -4286,7 +4292,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Saudi Arabia Workbook"/>
@@ -4917,7 +4923,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Iran Workbook"/>
@@ -5548,7 +5554,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Tanzania Workbook"/>
@@ -6179,7 +6185,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Zambia Workbook"/>
@@ -7131,20 +7137,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I223"/>
+  <dimension ref="A1:J223"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J223"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.875" style="1"/>
-    <col min="3" max="8" width="10.875" style="2"/>
-    <col min="9" max="9" width="10.875" style="1"/>
+    <col min="1" max="2" width="11" style="1"/>
+    <col min="3" max="8" width="11" style="2"/>
+    <col min="9" max="9" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="str">
         <f>[1]USData!A1</f>
         <v>Year</v>
@@ -7180,8 +7186,11 @@
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <f>[1]USData!A2</f>
         <v>1980</v>
@@ -7218,8 +7227,11 @@
         <f>[1]USData!I2</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <f>[1]USData!A3</f>
         <v>1981</v>
@@ -7256,8 +7268,11 @@
         <f>[1]USData!I3</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <f>[1]USData!A4</f>
         <v>1982</v>
@@ -7294,8 +7309,11 @@
         <f>[1]USData!I4</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <f>[1]USData!A5</f>
         <v>1983</v>
@@ -7332,8 +7350,11 @@
         <f>[1]USData!I5</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <f>[1]USData!A6</f>
         <v>1984</v>
@@ -7370,8 +7391,11 @@
         <f>[1]USData!I6</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <f>[1]USData!A7</f>
         <v>1985</v>
@@ -7408,8 +7432,11 @@
         <f>[1]USData!I7</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <f>[1]USData!A8</f>
         <v>1986</v>
@@ -7446,8 +7473,11 @@
         <f>[1]USData!I8</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <f>[1]USData!A9</f>
         <v>1987</v>
@@ -7484,8 +7514,11 @@
         <f>[1]USData!I9</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <f>[1]USData!A10</f>
         <v>1988</v>
@@ -7522,8 +7555,11 @@
         <f>[1]USData!I10</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <f>[1]USData!A11</f>
         <v>1989</v>
@@ -7560,8 +7596,11 @@
         <f>[1]USData!I11</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <f>[1]USData!A12</f>
         <v>1990</v>
@@ -7598,8 +7637,11 @@
         <f>[1]USData!I12</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <f>[1]USData!A13</f>
         <v>1991</v>
@@ -7636,8 +7678,11 @@
         <f>[1]USData!I13</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <f>[1]USData!A14</f>
         <v>1992</v>
@@ -7674,8 +7719,11 @@
         <f>[1]USData!I14</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <f>[1]USData!A15</f>
         <v>1993</v>
@@ -7712,8 +7760,11 @@
         <f>[1]USData!I15</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <f>[1]USData!A16</f>
         <v>1994</v>
@@ -7750,8 +7801,11 @@
         <f>[1]USData!I16</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <f>[1]USData!A17</f>
         <v>1995</v>
@@ -7788,8 +7842,11 @@
         <f>[1]USData!I17</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <f>[1]USData!A18</f>
         <v>1996</v>
@@ -7826,8 +7883,11 @@
         <f>[1]USData!I18</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <f>[1]USData!A19</f>
         <v>1997</v>
@@ -7864,8 +7924,11 @@
         <f>[1]USData!I19</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <f>[1]USData!A20</f>
         <v>1998</v>
@@ -7902,8 +7965,11 @@
         <f>[1]USData!I20</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <f>[1]USData!A21</f>
         <v>1999</v>
@@ -7940,8 +8006,11 @@
         <f>[1]USData!I21</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <f>[1]USData!A22</f>
         <v>2000</v>
@@ -7978,8 +8047,11 @@
         <f>[1]USData!I22</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <f>[1]USData!A23</f>
         <v>2001</v>
@@ -8016,8 +8088,11 @@
         <f>[1]USData!I23</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <f>[1]USData!A24</f>
         <v>2002</v>
@@ -8054,8 +8129,11 @@
         <f>[1]USData!I24</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <f>[1]USData!A25</f>
         <v>2003</v>
@@ -8092,8 +8170,11 @@
         <f>[1]USData!I25</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <f>[1]USData!A26</f>
         <v>2004</v>
@@ -8130,8 +8211,11 @@
         <f>[1]USData!I26</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <f>[1]USData!A27</f>
         <v>2005</v>
@@ -8168,8 +8252,11 @@
         <f>[1]USData!I27</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <f>[1]USData!A28</f>
         <v>2006</v>
@@ -8206,8 +8293,11 @@
         <f>[1]USData!I28</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <f>[1]USData!A29</f>
         <v>2007</v>
@@ -8244,8 +8334,11 @@
         <f>[1]USData!I29</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <f>[1]USData!A30</f>
         <v>2008</v>
@@ -8282,8 +8375,11 @@
         <f>[1]USData!I30</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <f>[1]USData!A31</f>
         <v>2009</v>
@@ -8320,8 +8416,11 @@
         <f>[1]USData!I31</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <f>[1]USData!A32</f>
         <v>2010</v>
@@ -8358,8 +8457,11 @@
         <f>[1]USData!I32</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <f>[1]USData!A33</f>
         <v>2011</v>
@@ -8396,8 +8498,11 @@
         <f>[1]USData!I33</f>
         <v>US</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <f>[2]UKData!A2</f>
         <v>1980</v>
@@ -8434,8 +8539,11 @@
         <f>[2]UKData!I2</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <f>[2]UKData!A3</f>
         <v>1981</v>
@@ -8472,8 +8580,11 @@
         <f>[2]UKData!I3</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <f>[2]UKData!A4</f>
         <v>1982</v>
@@ -8510,8 +8621,11 @@
         <f>[2]UKData!I4</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <f>[2]UKData!A5</f>
         <v>1983</v>
@@ -8548,8 +8662,11 @@
         <f>[2]UKData!I5</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <f>[2]UKData!A6</f>
         <v>1984</v>
@@ -8586,8 +8703,11 @@
         <f>[2]UKData!I6</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="1">
         <f>[2]UKData!A7</f>
         <v>1985</v>
@@ -8624,8 +8744,11 @@
         <f>[2]UKData!I7</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="1">
         <f>[2]UKData!A8</f>
         <v>1986</v>
@@ -8662,8 +8785,11 @@
         <f>[2]UKData!I8</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="1">
         <f>[2]UKData!A9</f>
         <v>1987</v>
@@ -8700,8 +8826,11 @@
         <f>[2]UKData!I9</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" s="1">
         <f>[2]UKData!A10</f>
         <v>1988</v>
@@ -8738,8 +8867,11 @@
         <f>[2]UKData!I10</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="1">
         <f>[2]UKData!A11</f>
         <v>1989</v>
@@ -8776,8 +8908,11 @@
         <f>[2]UKData!I11</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="1">
         <f>[2]UKData!A12</f>
         <v>1990</v>
@@ -8814,8 +8949,11 @@
         <f>[2]UKData!I12</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="1">
         <f>[2]UKData!A13</f>
         <v>1991</v>
@@ -8852,8 +8990,11 @@
         <f>[2]UKData!I13</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="1">
         <f>[2]UKData!A14</f>
         <v>1992</v>
@@ -8890,8 +9031,11 @@
         <f>[2]UKData!I14</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="1">
         <f>[2]UKData!A15</f>
         <v>1993</v>
@@ -8928,8 +9072,11 @@
         <f>[2]UKData!I15</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="1">
         <f>[2]UKData!A16</f>
         <v>1994</v>
@@ -8966,8 +9113,11 @@
         <f>[2]UKData!I16</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="1">
         <f>[2]UKData!A17</f>
         <v>1995</v>
@@ -9004,8 +9154,11 @@
         <f>[2]UKData!I17</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="1">
         <f>[2]UKData!A18</f>
         <v>1996</v>
@@ -9042,8 +9195,11 @@
         <f>[2]UKData!I18</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="1">
         <f>[2]UKData!A19</f>
         <v>1997</v>
@@ -9080,8 +9236,11 @@
         <f>[2]UKData!I19</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="1">
         <f>[2]UKData!A20</f>
         <v>1998</v>
@@ -9118,8 +9277,11 @@
         <f>[2]UKData!I20</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="1">
         <f>[2]UKData!A21</f>
         <v>1999</v>
@@ -9156,8 +9318,11 @@
         <f>[2]UKData!I21</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="1">
         <f>[2]UKData!A22</f>
         <v>2000</v>
@@ -9194,8 +9359,11 @@
         <f>[2]UKData!I22</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="1">
         <f>[2]UKData!A23</f>
         <v>2001</v>
@@ -9232,8 +9400,11 @@
         <f>[2]UKData!I23</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="1">
         <f>[2]UKData!A24</f>
         <v>2002</v>
@@ -9270,8 +9441,11 @@
         <f>[2]UKData!I24</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="1">
         <f>[2]UKData!A25</f>
         <v>2003</v>
@@ -9308,8 +9482,11 @@
         <f>[2]UKData!I25</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="1">
         <f>[2]UKData!A26</f>
         <v>2004</v>
@@ -9346,8 +9523,11 @@
         <f>[2]UKData!I26</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="1">
         <f>[2]UKData!A27</f>
         <v>2005</v>
@@ -9384,8 +9564,11 @@
         <f>[2]UKData!I27</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="1">
         <f>[2]UKData!A28</f>
         <v>2006</v>
@@ -9422,8 +9605,11 @@
         <f>[2]UKData!I28</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="1">
         <f>[2]UKData!A29</f>
         <v>2007</v>
@@ -9460,8 +9646,11 @@
         <f>[2]UKData!I29</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="1">
         <f>[2]UKData!A30</f>
         <v>2008</v>
@@ -9498,8 +9687,11 @@
         <f>[2]UKData!I30</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="1">
         <f>[2]UKData!A31</f>
         <v>2009</v>
@@ -9536,8 +9728,11 @@
         <f>[2]UKData!I31</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="1">
         <f>[2]UKData!A32</f>
         <v>2010</v>
@@ -9574,8 +9769,11 @@
         <f>[2]UKData!I32</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <f>[2]UKData!A33</f>
         <v>2011</v>
@@ -9612,8 +9810,11 @@
         <f>[2]UKData!I33</f>
         <v>UK</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <f>[3]JPData!A2</f>
         <v>1980</v>
@@ -9650,8 +9851,11 @@
         <f>[3]JPData!I2</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <f>[3]JPData!A3</f>
         <v>1981</v>
@@ -9688,8 +9892,11 @@
         <f>[3]JPData!I3</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <f>[3]JPData!A4</f>
         <v>1982</v>
@@ -9726,8 +9933,11 @@
         <f>[3]JPData!I4</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <f>[3]JPData!A5</f>
         <v>1983</v>
@@ -9764,8 +9974,11 @@
         <f>[3]JPData!I5</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <f>[3]JPData!A6</f>
         <v>1984</v>
@@ -9802,8 +10015,11 @@
         <f>[3]JPData!I6</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <f>[3]JPData!A7</f>
         <v>1985</v>
@@ -9840,8 +10056,11 @@
         <f>[3]JPData!I7</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <f>[3]JPData!A8</f>
         <v>1986</v>
@@ -9878,8 +10097,11 @@
         <f>[3]JPData!I8</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <f>[3]JPData!A9</f>
         <v>1987</v>
@@ -9916,8 +10138,11 @@
         <f>[3]JPData!I9</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <f>[3]JPData!A10</f>
         <v>1988</v>
@@ -9954,8 +10179,11 @@
         <f>[3]JPData!I10</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <f>[3]JPData!A11</f>
         <v>1989</v>
@@ -9992,8 +10220,11 @@
         <f>[3]JPData!I11</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <f>[3]JPData!A12</f>
         <v>1990</v>
@@ -10030,8 +10261,11 @@
         <f>[3]JPData!I12</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <f>[3]JPData!A13</f>
         <v>1991</v>
@@ -10068,8 +10302,11 @@
         <f>[3]JPData!I13</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <f>[3]JPData!A14</f>
         <v>1992</v>
@@ -10106,8 +10343,11 @@
         <f>[3]JPData!I14</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <f>[3]JPData!A15</f>
         <v>1993</v>
@@ -10144,8 +10384,11 @@
         <f>[3]JPData!I15</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <f>[3]JPData!A16</f>
         <v>1994</v>
@@ -10182,8 +10425,11 @@
         <f>[3]JPData!I16</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <f>[3]JPData!A17</f>
         <v>1995</v>
@@ -10220,8 +10466,11 @@
         <f>[3]JPData!I17</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <f>[3]JPData!A18</f>
         <v>1996</v>
@@ -10258,8 +10507,11 @@
         <f>[3]JPData!I18</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <f>[3]JPData!A19</f>
         <v>1997</v>
@@ -10296,8 +10548,11 @@
         <f>[3]JPData!I19</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <f>[3]JPData!A20</f>
         <v>1998</v>
@@ -10334,8 +10589,11 @@
         <f>[3]JPData!I20</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <f>[3]JPData!A21</f>
         <v>1999</v>
@@ -10372,8 +10630,11 @@
         <f>[3]JPData!I21</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <f>[3]JPData!A22</f>
         <v>2000</v>
@@ -10410,8 +10671,11 @@
         <f>[3]JPData!I22</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <f>[3]JPData!A23</f>
         <v>2001</v>
@@ -10448,8 +10712,11 @@
         <f>[3]JPData!I23</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <f>[3]JPData!A24</f>
         <v>2002</v>
@@ -10486,8 +10753,11 @@
         <f>[3]JPData!I24</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <f>[3]JPData!A25</f>
         <v>2003</v>
@@ -10524,8 +10794,11 @@
         <f>[3]JPData!I25</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <f>[3]JPData!A26</f>
         <v>2004</v>
@@ -10562,8 +10835,11 @@
         <f>[3]JPData!I26</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <f>[3]JPData!A27</f>
         <v>2005</v>
@@ -10600,8 +10876,11 @@
         <f>[3]JPData!I27</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <f>[3]JPData!A28</f>
         <v>2006</v>
@@ -10638,8 +10917,11 @@
         <f>[3]JPData!I28</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <f>[3]JPData!A29</f>
         <v>2007</v>
@@ -10676,8 +10958,11 @@
         <f>[3]JPData!I29</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <f>[3]JPData!A30</f>
         <v>2008</v>
@@ -10714,8 +10999,11 @@
         <f>[3]JPData!I30</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <f>[3]JPData!A31</f>
         <v>2009</v>
@@ -10752,8 +11040,11 @@
         <f>[3]JPData!I31</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <f>[3]JPData!A32</f>
         <v>2010</v>
@@ -10790,8 +11081,11 @@
         <f>[3]JPData!I32</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <f>[3]JPData!A33</f>
         <v>2011</v>
@@ -10828,8 +11122,11 @@
         <f>[3]JPData!I33</f>
         <v>JP</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <f>[4]CNData!A2</f>
         <v>1991</v>
@@ -10866,8 +11163,11 @@
         <f>[4]CNData!I2</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <f>[4]CNData!A3</f>
         <v>1992</v>
@@ -10904,8 +11204,11 @@
         <f>[4]CNData!I3</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <f>[4]CNData!A4</f>
         <v>1993</v>
@@ -10942,8 +11245,11 @@
         <f>[4]CNData!I4</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <f>[4]CNData!A5</f>
         <v>1994</v>
@@ -10980,8 +11286,11 @@
         <f>[4]CNData!I5</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <f>[4]CNData!A6</f>
         <v>1995</v>
@@ -11018,8 +11327,11 @@
         <f>[4]CNData!I6</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <f>[4]CNData!A7</f>
         <v>1996</v>
@@ -11056,8 +11368,11 @@
         <f>[4]CNData!I7</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <f>[4]CNData!A8</f>
         <v>1997</v>
@@ -11094,8 +11409,11 @@
         <f>[4]CNData!I8</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <f>[4]CNData!A9</f>
         <v>1998</v>
@@ -11132,8 +11450,11 @@
         <f>[4]CNData!I9</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <f>[4]CNData!A10</f>
         <v>1999</v>
@@ -11170,8 +11491,11 @@
         <f>[4]CNData!I10</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <f>[4]CNData!A11</f>
         <v>2000</v>
@@ -11208,8 +11532,11 @@
         <f>[4]CNData!I11</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <f>[4]CNData!A12</f>
         <v>2001</v>
@@ -11246,8 +11573,11 @@
         <f>[4]CNData!I12</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <f>[4]CNData!A13</f>
         <v>2002</v>
@@ -11284,8 +11614,11 @@
         <f>[4]CNData!I13</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <f>[4]CNData!A14</f>
         <v>2003</v>
@@ -11322,8 +11655,11 @@
         <f>[4]CNData!I14</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <f>[4]CNData!A15</f>
         <v>2004</v>
@@ -11360,8 +11696,11 @@
         <f>[4]CNData!I15</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <f>[4]CNData!A16</f>
         <v>2005</v>
@@ -11398,8 +11737,11 @@
         <f>[4]CNData!I16</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <f>[4]CNData!A17</f>
         <v>2006</v>
@@ -11436,8 +11778,11 @@
         <f>[4]CNData!I17</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <f>[4]CNData!A18</f>
         <v>2007</v>
@@ -11474,8 +11819,11 @@
         <f>[4]CNData!I18</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <f>[4]CNData!A19</f>
         <v>2008</v>
@@ -11512,8 +11860,11 @@
         <f>[4]CNData!I19</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <f>[4]CNData!A20</f>
         <v>2009</v>
@@ -11550,8 +11901,11 @@
         <f>[4]CNData!I20</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <f>[4]CNData!A21</f>
         <v>2010</v>
@@ -11588,8 +11942,11 @@
         <f>[4]CNData!I21</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <f>[4]CNData!A22</f>
         <v>2011</v>
@@ -11626,8 +11983,11 @@
         <f>[4]CNData!I22</f>
         <v>CN</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <f>[5]ZAData!A2</f>
         <v>1991</v>
@@ -11664,8 +12024,11 @@
         <f>[5]ZAData!I2</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <f>[5]ZAData!A3</f>
         <v>1992</v>
@@ -11702,8 +12065,11 @@
         <f>[5]ZAData!I3</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <f>[5]ZAData!A4</f>
         <v>1993</v>
@@ -11740,8 +12106,11 @@
         <f>[5]ZAData!I4</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <f>[5]ZAData!A5</f>
         <v>1994</v>
@@ -11778,8 +12147,11 @@
         <f>[5]ZAData!I5</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <f>[5]ZAData!A6</f>
         <v>1995</v>
@@ -11816,8 +12188,11 @@
         <f>[5]ZAData!I6</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <f>[5]ZAData!A7</f>
         <v>1996</v>
@@ -11854,8 +12229,11 @@
         <f>[5]ZAData!I7</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <f>[5]ZAData!A8</f>
         <v>1997</v>
@@ -11892,8 +12270,11 @@
         <f>[5]ZAData!I8</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <f>[5]ZAData!A9</f>
         <v>1998</v>
@@ -11930,8 +12311,11 @@
         <f>[5]ZAData!I9</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <f>[5]ZAData!A10</f>
         <v>1999</v>
@@ -11968,8 +12352,11 @@
         <f>[5]ZAData!I10</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <f>[5]ZAData!A11</f>
         <v>2000</v>
@@ -12006,8 +12393,11 @@
         <f>[5]ZAData!I11</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <f>[5]ZAData!A12</f>
         <v>2001</v>
@@ -12044,8 +12434,11 @@
         <f>[5]ZAData!I12</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <f>[5]ZAData!A13</f>
         <v>2002</v>
@@ -12082,8 +12475,11 @@
         <f>[5]ZAData!I13</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <f>[5]ZAData!A14</f>
         <v>2003</v>
@@ -12120,8 +12516,11 @@
         <f>[5]ZAData!I14</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <f>[5]ZAData!A15</f>
         <v>2004</v>
@@ -12158,8 +12557,11 @@
         <f>[5]ZAData!I15</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <f>[5]ZAData!A16</f>
         <v>2005</v>
@@ -12196,8 +12598,11 @@
         <f>[5]ZAData!I16</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <f>[5]ZAData!A17</f>
         <v>2006</v>
@@ -12234,8 +12639,11 @@
         <f>[5]ZAData!I17</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <f>[5]ZAData!A18</f>
         <v>2007</v>
@@ -12272,8 +12680,11 @@
         <f>[5]ZAData!I18</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <f>[5]ZAData!A19</f>
         <v>2008</v>
@@ -12310,8 +12721,11 @@
         <f>[5]ZAData!I19</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <f>[5]ZAData!A20</f>
         <v>2009</v>
@@ -12348,8 +12762,11 @@
         <f>[5]ZAData!I20</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <f>[5]ZAData!A21</f>
         <v>2010</v>
@@ -12386,8 +12803,11 @@
         <f>[5]ZAData!I21</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <f>[5]ZAData!A22</f>
         <v>2011</v>
@@ -12424,8 +12844,11 @@
         <f>[5]ZAData!I22</f>
         <v>ZA</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <f>[6]SAData!A2</f>
         <v>1991</v>
@@ -12462,8 +12885,11 @@
         <f>[6]SAData!I2</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <f>[6]SAData!A3</f>
         <v>1992</v>
@@ -12500,8 +12926,11 @@
         <f>[6]SAData!I3</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <f>[6]SAData!A4</f>
         <v>1993</v>
@@ -12538,8 +12967,11 @@
         <f>[6]SAData!I4</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <f>[6]SAData!A5</f>
         <v>1994</v>
@@ -12576,8 +13008,11 @@
         <f>[6]SAData!I5</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <f>[6]SAData!A6</f>
         <v>1995</v>
@@ -12614,8 +13049,11 @@
         <f>[6]SAData!I6</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <f>[6]SAData!A7</f>
         <v>1996</v>
@@ -12652,8 +13090,11 @@
         <f>[6]SAData!I7</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <f>[6]SAData!A8</f>
         <v>1997</v>
@@ -12690,8 +13131,11 @@
         <f>[6]SAData!I8</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <f>[6]SAData!A9</f>
         <v>1998</v>
@@ -12728,8 +13172,11 @@
         <f>[6]SAData!I9</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <f>[6]SAData!A10</f>
         <v>1999</v>
@@ -12766,8 +13213,11 @@
         <f>[6]SAData!I10</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <f>[6]SAData!A11</f>
         <v>2000</v>
@@ -12804,8 +13254,11 @@
         <f>[6]SAData!I11</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J149" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <f>[6]SAData!A12</f>
         <v>2001</v>
@@ -12842,8 +13295,11 @@
         <f>[6]SAData!I12</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J150" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <f>[6]SAData!A13</f>
         <v>2002</v>
@@ -12880,8 +13336,11 @@
         <f>[6]SAData!I13</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J151" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <f>[6]SAData!A14</f>
         <v>2003</v>
@@ -12918,8 +13377,11 @@
         <f>[6]SAData!I14</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <f>[6]SAData!A15</f>
         <v>2004</v>
@@ -12956,8 +13418,11 @@
         <f>[6]SAData!I15</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <f>[6]SAData!A16</f>
         <v>2005</v>
@@ -12994,8 +13459,11 @@
         <f>[6]SAData!I16</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J154" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <f>[6]SAData!A17</f>
         <v>2006</v>
@@ -13032,8 +13500,11 @@
         <f>[6]SAData!I17</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J155" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <f>[6]SAData!A18</f>
         <v>2007</v>
@@ -13070,8 +13541,11 @@
         <f>[6]SAData!I18</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <f>[6]SAData!A19</f>
         <v>2008</v>
@@ -13108,8 +13582,11 @@
         <f>[6]SAData!I19</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <f>[6]SAData!A20</f>
         <v>2009</v>
@@ -13146,8 +13623,11 @@
         <f>[6]SAData!I20</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <f>[6]SAData!A21</f>
         <v>2010</v>
@@ -13184,8 +13664,11 @@
         <f>[6]SAData!I21</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J159" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <f>[6]SAData!A22</f>
         <v>2011</v>
@@ -13222,8 +13705,11 @@
         <f>[6]SAData!I22</f>
         <v>SA</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J160" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <f>[7]IRData!A2</f>
         <v>1991</v>
@@ -13260,8 +13746,11 @@
         <f>[7]IRData!I2</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J161" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <f>[7]IRData!A3</f>
         <v>1992</v>
@@ -13298,8 +13787,11 @@
         <f>[7]IRData!I3</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J162" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <f>[7]IRData!A4</f>
         <v>1993</v>
@@ -13336,8 +13828,11 @@
         <f>[7]IRData!I4</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J163" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <f>[7]IRData!A5</f>
         <v>1994</v>
@@ -13374,8 +13869,11 @@
         <f>[7]IRData!I5</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J164" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <f>[7]IRData!A6</f>
         <v>1995</v>
@@ -13412,8 +13910,11 @@
         <f>[7]IRData!I6</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J165" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <f>[7]IRData!A7</f>
         <v>1996</v>
@@ -13450,8 +13951,11 @@
         <f>[7]IRData!I7</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J166" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <f>[7]IRData!A8</f>
         <v>1997</v>
@@ -13488,8 +13992,11 @@
         <f>[7]IRData!I8</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J167" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <f>[7]IRData!A9</f>
         <v>1998</v>
@@ -13526,8 +14033,11 @@
         <f>[7]IRData!I9</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J168" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <f>[7]IRData!A10</f>
         <v>1999</v>
@@ -13564,8 +14074,11 @@
         <f>[7]IRData!I10</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <f>[7]IRData!A11</f>
         <v>2000</v>
@@ -13602,8 +14115,11 @@
         <f>[7]IRData!I11</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J170" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <f>[7]IRData!A12</f>
         <v>2001</v>
@@ -13640,8 +14156,11 @@
         <f>[7]IRData!I12</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J171" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <f>[7]IRData!A13</f>
         <v>2002</v>
@@ -13678,8 +14197,11 @@
         <f>[7]IRData!I13</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J172" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <f>[7]IRData!A14</f>
         <v>2003</v>
@@ -13716,8 +14238,11 @@
         <f>[7]IRData!I14</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J173" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <f>[7]IRData!A15</f>
         <v>2004</v>
@@ -13754,8 +14279,11 @@
         <f>[7]IRData!I15</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J174" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <f>[7]IRData!A16</f>
         <v>2005</v>
@@ -13792,8 +14320,11 @@
         <f>[7]IRData!I16</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J175" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <f>[7]IRData!A17</f>
         <v>2006</v>
@@ -13830,8 +14361,11 @@
         <f>[7]IRData!I17</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J176" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10">
       <c r="A177" s="1">
         <f>[7]IRData!A18</f>
         <v>2007</v>
@@ -13868,8 +14402,11 @@
         <f>[7]IRData!I18</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J177" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10">
       <c r="A178" s="1">
         <f>[7]IRData!A19</f>
         <v>2008</v>
@@ -13906,8 +14443,11 @@
         <f>[7]IRData!I19</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J178" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10">
       <c r="A179" s="1">
         <f>[7]IRData!A20</f>
         <v>2009</v>
@@ -13944,8 +14484,11 @@
         <f>[7]IRData!I20</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J179" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10">
       <c r="A180" s="1">
         <f>[7]IRData!A21</f>
         <v>2010</v>
@@ -13982,8 +14525,11 @@
         <f>[7]IRData!I21</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J180" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10">
       <c r="A181" s="1">
         <f>[7]IRData!A22</f>
         <v>2011</v>
@@ -14020,8 +14566,11 @@
         <f>[7]IRData!I22</f>
         <v>IR</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J181" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10">
       <c r="A182" s="1">
         <f>[8]TZData!A2</f>
         <v>1991</v>
@@ -14058,8 +14607,11 @@
         <f>[8]TZData!I2</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J182" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10">
       <c r="A183" s="1">
         <f>[8]TZData!A3</f>
         <v>1992</v>
@@ -14096,8 +14648,11 @@
         <f>[8]TZData!I3</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J183" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10">
       <c r="A184" s="1">
         <f>[8]TZData!A4</f>
         <v>1993</v>
@@ -14134,8 +14689,11 @@
         <f>[8]TZData!I4</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J184" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10">
       <c r="A185" s="1">
         <f>[8]TZData!A5</f>
         <v>1994</v>
@@ -14172,8 +14730,11 @@
         <f>[8]TZData!I5</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J185" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10">
       <c r="A186" s="1">
         <f>[8]TZData!A6</f>
         <v>1995</v>
@@ -14210,8 +14771,11 @@
         <f>[8]TZData!I6</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J186" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10">
       <c r="A187" s="1">
         <f>[8]TZData!A7</f>
         <v>1996</v>
@@ -14248,8 +14812,11 @@
         <f>[8]TZData!I7</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J187" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10">
       <c r="A188" s="1">
         <f>[8]TZData!A8</f>
         <v>1997</v>
@@ -14286,8 +14853,11 @@
         <f>[8]TZData!I8</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J188" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10">
       <c r="A189" s="1">
         <f>[8]TZData!A9</f>
         <v>1998</v>
@@ -14324,8 +14894,11 @@
         <f>[8]TZData!I9</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J189" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10">
       <c r="A190" s="1">
         <f>[8]TZData!A10</f>
         <v>1999</v>
@@ -14362,8 +14935,11 @@
         <f>[8]TZData!I10</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J190" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10">
       <c r="A191" s="1">
         <f>[8]TZData!A11</f>
         <v>2000</v>
@@ -14400,8 +14976,11 @@
         <f>[8]TZData!I11</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J191" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10">
       <c r="A192" s="1">
         <f>[8]TZData!A12</f>
         <v>2001</v>
@@ -14438,8 +15017,11 @@
         <f>[8]TZData!I12</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J192" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10">
       <c r="A193" s="1">
         <f>[8]TZData!A13</f>
         <v>2002</v>
@@ -14476,8 +15058,11 @@
         <f>[8]TZData!I13</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J193" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10">
       <c r="A194" s="1">
         <f>[8]TZData!A14</f>
         <v>2003</v>
@@ -14514,8 +15099,11 @@
         <f>[8]TZData!I14</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J194" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10">
       <c r="A195" s="1">
         <f>[8]TZData!A15</f>
         <v>2004</v>
@@ -14552,8 +15140,11 @@
         <f>[8]TZData!I15</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J195" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10">
       <c r="A196" s="1">
         <f>[8]TZData!A16</f>
         <v>2005</v>
@@ -14590,8 +15181,11 @@
         <f>[8]TZData!I16</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J196" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10">
       <c r="A197" s="1">
         <f>[8]TZData!A17</f>
         <v>2006</v>
@@ -14628,8 +15222,11 @@
         <f>[8]TZData!I17</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J197" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10">
       <c r="A198" s="1">
         <f>[8]TZData!A18</f>
         <v>2007</v>
@@ -14666,8 +15263,11 @@
         <f>[8]TZData!I18</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J198" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10">
       <c r="A199" s="1">
         <f>[8]TZData!A19</f>
         <v>2008</v>
@@ -14704,8 +15304,11 @@
         <f>[8]TZData!I19</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J199" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10">
       <c r="A200" s="1">
         <f>[8]TZData!A20</f>
         <v>2009</v>
@@ -14742,8 +15345,11 @@
         <f>[8]TZData!I20</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J200" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10">
       <c r="A201" s="1">
         <f>[8]TZData!A21</f>
         <v>2010</v>
@@ -14780,8 +15386,11 @@
         <f>[8]TZData!I21</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J201" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10">
       <c r="A202" s="1">
         <f>[8]TZData!A22</f>
         <v>2011</v>
@@ -14818,8 +15427,11 @@
         <f>[8]TZData!I22</f>
         <v>TZ</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J202" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10">
       <c r="A203" s="1">
         <f>[9]ZMData!A2</f>
         <v>1991</v>
@@ -14856,8 +15468,11 @@
         <f>[9]ZMData!I2</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J203" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10">
       <c r="A204" s="1">
         <f>[9]ZMData!A3</f>
         <v>1992</v>
@@ -14894,8 +15509,11 @@
         <f>[9]ZMData!I3</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J204" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10">
       <c r="A205" s="1">
         <f>[9]ZMData!A4</f>
         <v>1993</v>
@@ -14932,8 +15550,11 @@
         <f>[9]ZMData!I4</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J205" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10">
       <c r="A206" s="1">
         <f>[9]ZMData!A5</f>
         <v>1994</v>
@@ -14970,8 +15591,11 @@
         <f>[9]ZMData!I5</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J206" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10">
       <c r="A207" s="1">
         <f>[9]ZMData!A6</f>
         <v>1995</v>
@@ -15008,8 +15632,11 @@
         <f>[9]ZMData!I6</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J207" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10">
       <c r="A208" s="1">
         <f>[9]ZMData!A7</f>
         <v>1996</v>
@@ -15046,8 +15673,11 @@
         <f>[9]ZMData!I7</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J208" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10">
       <c r="A209" s="1">
         <f>[9]ZMData!A8</f>
         <v>1997</v>
@@ -15084,8 +15714,11 @@
         <f>[9]ZMData!I8</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J209" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10">
       <c r="A210" s="1">
         <f>[9]ZMData!A9</f>
         <v>1998</v>
@@ -15122,8 +15755,11 @@
         <f>[9]ZMData!I9</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J210" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10">
       <c r="A211" s="1">
         <f>[9]ZMData!A10</f>
         <v>1999</v>
@@ -15160,8 +15796,11 @@
         <f>[9]ZMData!I10</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J211" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10">
       <c r="A212" s="1">
         <f>[9]ZMData!A11</f>
         <v>2000</v>
@@ -15198,8 +15837,11 @@
         <f>[9]ZMData!I11</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J212" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10">
       <c r="A213" s="1">
         <f>[9]ZMData!A12</f>
         <v>2001</v>
@@ -15236,8 +15878,11 @@
         <f>[9]ZMData!I12</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J213" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10">
       <c r="A214" s="1">
         <f>[9]ZMData!A13</f>
         <v>2002</v>
@@ -15274,8 +15919,11 @@
         <f>[9]ZMData!I13</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J214" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10">
       <c r="A215" s="1">
         <f>[9]ZMData!A14</f>
         <v>2003</v>
@@ -15312,8 +15960,11 @@
         <f>[9]ZMData!I14</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J215" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10">
       <c r="A216" s="1">
         <f>[9]ZMData!A15</f>
         <v>2004</v>
@@ -15350,8 +16001,11 @@
         <f>[9]ZMData!I15</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J216" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10">
       <c r="A217" s="1">
         <f>[9]ZMData!A16</f>
         <v>2005</v>
@@ -15388,8 +16042,11 @@
         <f>[9]ZMData!I16</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J217" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10">
       <c r="A218" s="1">
         <f>[9]ZMData!A17</f>
         <v>2006</v>
@@ -15426,8 +16083,11 @@
         <f>[9]ZMData!I17</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J218" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10">
       <c r="A219" s="1">
         <f>[9]ZMData!A18</f>
         <v>2007</v>
@@ -15464,8 +16124,11 @@
         <f>[9]ZMData!I18</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J219" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10">
       <c r="A220" s="1">
         <f>[9]ZMData!A19</f>
         <v>2008</v>
@@ -15502,8 +16165,11 @@
         <f>[9]ZMData!I19</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J220" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10">
       <c r="A221" s="1">
         <f>[9]ZMData!A20</f>
         <v>2009</v>
@@ -15540,8 +16206,11 @@
         <f>[9]ZMData!I20</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J221" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10">
       <c r="A222" s="1">
         <f>[9]ZMData!A21</f>
         <v>2010</v>
@@ -15578,8 +16247,11 @@
         <f>[9]ZMData!I21</f>
         <v>ZM</v>
       </c>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J222" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10">
       <c r="A223" s="1">
         <f>[9]ZMData!A22</f>
         <v>2011</v>
@@ -15615,6 +16287,9 @@
       <c r="I223" s="1" t="str">
         <f>[9]ZMData!I22</f>
         <v>ZM</v>
+      </c>
+      <c r="J223" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>